<commit_message>
Tir limite a 5
TIr qui se limite a 5 (peut etre modifier) debut de la colision
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f03a1208622c5793/Bureau/L3/jeux/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\jeux\gamesJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CD2AD61-9D9C-4A26-9606-5815532EF03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903EFB00-3025-4B69-87D7-07E736C3D902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,12 +68,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Sous-tâche 2</t>
-  </si>
-  <si>
-    <t>Sous-tâche 3</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>Instancier un objet à ces coordonées</t>
+  </si>
+  <si>
+    <t>rebond de la balle</t>
+  </si>
+  <si>
+    <t>direction de la balle</t>
   </si>
 </sst>
 </file>
@@ -468,6 +468,15 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -494,15 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,7 +1014,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1031,69 +1031,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="A1" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="G1" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:67" ht="12" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="G2" s="3">
         <f ca="1">TODAY()</f>
-        <v>43770</v>
+        <v>43781</v>
       </c>
     </row>
     <row r="3" spans="1:67" ht="12" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="A3" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:67" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="26"/>
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:67" ht="12" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="35" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="35" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="33"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:67" ht="12" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="44"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="30">
         <v>43770</v>
       </c>
@@ -1102,13 +1102,13 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:67" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
+      <c r="A7" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="18"/>
       <c r="G7" s="15"/>
       <c r="H7" s="5">
@@ -1599,20 +1599,20 @@
     </row>
     <row r="9" spans="1:67" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="48" t="s">
+      <c r="B9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="47" t="s">
-        <v>20</v>
+      <c r="F9" s="38" t="s">
+        <v>18</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="10" t="str">
@@ -1858,11 +1858,11 @@
     </row>
     <row r="10" spans="1:67" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="47"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="17"/>
       <c r="H10" s="10">
         <f>DAY(H7)</f>
@@ -2110,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="23"/>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="12" spans="1:67" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="36">
         <v>43770</v>
@@ -2196,10 +2196,10 @@
         <v>43770</v>
       </c>
       <c r="F12" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="20">
-        <f t="shared" ref="G12:G41" si="7">C12+F12*(E12-C12)</f>
+        <f t="shared" ref="G12:G22" si="7">C12+F12*(E12-C12)</f>
         <v>43770</v>
       </c>
       <c r="I12" s="3"/>
@@ -2264,27 +2264,27 @@
     </row>
     <row r="13" spans="1:67" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C13" s="36">
-        <v>43771</v>
+        <v>43773</v>
       </c>
       <c r="D13" s="13">
         <v>1</v>
       </c>
       <c r="E13" s="34">
         <f t="shared" ref="E13:E76" si="8">IF(B13="","",IF($C$5="OUI",WORKDAY(C13,IF(WEEKDAY(C13,2)&gt;=6,D13,D13-1)),C13+D13-1))</f>
-        <v>43771</v>
+        <v>43773</v>
       </c>
       <c r="F13" s="32">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G13" s="20">
         <f t="shared" si="7"/>
-        <v>43771</v>
+        <v>43773</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -2348,27 +2348,27 @@
     </row>
     <row r="14" spans="1:67" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C14" s="36">
-        <v>43772</v>
+        <v>43774</v>
       </c>
       <c r="D14" s="13">
         <v>1</v>
       </c>
       <c r="E14" s="34">
         <f t="shared" si="8"/>
-        <v>43772</v>
+        <v>43774</v>
       </c>
       <c r="F14" s="32">
         <v>0</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="7"/>
-        <v>43772</v>
+        <v>43774</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -2435,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="23"/>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="16" spans="1:67" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="37">
         <v>41530</v>
@@ -2517,8 +2517,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="34">
-        <f t="shared" si="8"/>
-        <v>41530</v>
+        <v>0</v>
       </c>
       <c r="F16" s="19">
         <v>0</v>
@@ -2530,10 +2529,10 @@
     </row>
     <row r="17" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="37">
         <v>41532</v>
@@ -2542,23 +2541,22 @@
         <v>12</v>
       </c>
       <c r="E17" s="34">
-        <f t="shared" si="8"/>
-        <v>41543</v>
+        <v>0</v>
       </c>
       <c r="F17" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G17" s="20">
         <f t="shared" si="7"/>
-        <v>41537.5</v>
+        <v>41532</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="37">
         <v>41548</v>
@@ -2567,11 +2565,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="34">
-        <f t="shared" si="8"/>
-        <v>41548</v>
+        <v>0</v>
       </c>
       <c r="F18" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="20">
         <f t="shared" si="7"/>
@@ -2580,10 +2577,10 @@
     </row>
     <row r="19" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="37">
         <v>41549</v>
@@ -2592,23 +2589,22 @@
         <v>6</v>
       </c>
       <c r="E19" s="34">
-        <f t="shared" si="8"/>
-        <v>41554</v>
+        <v>0</v>
       </c>
       <c r="F19" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="20">
         <f t="shared" si="7"/>
-        <v>41554</v>
+        <v>41549</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="37">
         <v>41555</v>
@@ -2617,8 +2613,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="34">
-        <f t="shared" si="8"/>
-        <v>41556</v>
+        <v>0</v>
       </c>
       <c r="G20" s="20">
         <f t="shared" si="7"/>
@@ -2627,10 +2622,10 @@
     </row>
     <row r="21" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="37">
         <v>41557</v>
@@ -2639,8 +2634,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="34">
-        <f t="shared" si="8"/>
-        <v>41574</v>
+        <v>0</v>
       </c>
       <c r="G21" s="20">
         <f t="shared" si="7"/>
@@ -2649,10 +2643,10 @@
     </row>
     <row r="22" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="37">
         <v>41575</v>
@@ -2661,8 +2655,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="34">
-        <f t="shared" si="8"/>
-        <v>41590</v>
+        <v>0</v>
       </c>
       <c r="G22" s="20">
         <f t="shared" si="7"/>
@@ -3152,11 +3145,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C2:E2"/>
@@ -3166,6 +3154,11 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="H8:BO8">
@@ -3279,7 +3272,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3290,7 +3283,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>